<commit_message>
⚒️Inclusão de funcionamento na IDE e na Build
</commit_message>
<xml_diff>
--- a/Backup/Qualificacao.xlsx
+++ b/Backup/Qualificacao.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Qualificação_Performance\Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\Qualificacao_Performance\Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A4105-9077-4D7C-BB31-F13D46DD35BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$B$1:$J$1621</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,86 +40,86 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - Log_alarmes" description="Conexão com a consulta 'Log_alarmes' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - Log_alarmes" description="Conexão com a consulta 'Log_alarmes' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Log_alarmes;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_alarmes]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Consulta - Log_salas" description="Conexão com a consulta 'Log_salas' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Consulta - Log_salas" description="Conexão com a consulta 'Log_salas' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Log_salas;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas]"/>
   </connection>
-  <connection id="3" keepAlive="1" name="Consulta - Log_salas - NIPO" description="Conexão com a consulta 'Log_salas - NIPO' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" keepAlive="1" name="Consulta - Log_salas - NIPO" description="Conexão com a consulta 'Log_salas - NIPO' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas - NIPO&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas - NIPO]"/>
   </connection>
-  <connection id="4" keepAlive="1" name="Consulta - Log_salas (1)" description="Conexão com a consulta 'Log_salas (1)' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" keepAlive="1" name="Consulta - Log_salas (1)" description="Conexão com a consulta 'Log_salas (1)' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (1)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (1)]"/>
   </connection>
-  <connection id="5" keepAlive="1" name="Consulta - Log_salas (10)" description="Conexão com a consulta 'Log_salas (10)' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" keepAlive="1" name="Consulta - Log_salas (10)" description="Conexão com a consulta 'Log_salas (10)' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (10)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (10)]"/>
   </connection>
-  <connection id="6" keepAlive="1" name="Consulta - Log_salas (11)" description="Conexão com a consulta 'Log_salas (11)' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" keepAlive="1" name="Consulta - Log_salas (11)" description="Conexão com a consulta 'Log_salas (11)' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (11)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (11)]"/>
   </connection>
-  <connection id="7" keepAlive="1" name="Consulta - Log_salas (12)" description="Ligação à consulta 'Log_salas (12)' no livro." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" keepAlive="1" name="Consulta - Log_salas (12)" description="Ligação à consulta 'Log_salas (12)' no livro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (12)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (12)]"/>
   </connection>
-  <connection id="8" keepAlive="1" name="Consulta - Log_salas (2)" description="Conexão com a consulta 'Log_salas (2)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" keepAlive="1" name="Consulta - Log_salas (2)" description="Conexão com a consulta 'Log_salas (2)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (2)]"/>
   </connection>
-  <connection id="9" keepAlive="1" name="Consulta - Log_salas (3)" description="Conexão com a consulta 'Log_salas (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" keepAlive="1" name="Consulta - Log_salas (3)" description="Conexão com a consulta 'Log_salas (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (3)]"/>
   </connection>
-  <connection id="10" keepAlive="1" name="Consulta - Log_salas (4)" description="Conexão com a consulta 'Log_salas (4)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" keepAlive="1" name="Consulta - Log_salas (4)" description="Conexão com a consulta 'Log_salas (4)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (4)]"/>
   </connection>
-  <connection id="11" keepAlive="1" name="Consulta - Log_salas (5)" description="Conexão com a consulta 'Log_salas (5)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" keepAlive="1" name="Consulta - Log_salas (5)" description="Conexão com a consulta 'Log_salas (5)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (5)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (5)]"/>
   </connection>
-  <connection id="12" keepAlive="1" name="Consulta - Log_salas (6)" description="Conexão com a consulta 'Log_salas (6)' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" keepAlive="1" name="Consulta - Log_salas (6)" description="Conexão com a consulta 'Log_salas (6)' na pasta de trabalho." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (6)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (6)]"/>
   </connection>
-  <connection id="13" keepAlive="1" name="Consulta - Log_salas (7)" description="Conexão com a consulta 'Log_salas (7)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="13" xr16:uid="{00000000-0015-0000-FFFF-FFFF0C000000}" keepAlive="1" name="Consulta - Log_salas (7)" description="Conexão com a consulta 'Log_salas (7)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (7)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (7)]"/>
   </connection>
-  <connection id="14" keepAlive="1" name="Consulta - Log_salas (8)" description="Conexão com a consulta 'Log_salas (8)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="14" xr16:uid="{00000000-0015-0000-FFFF-FFFF0D000000}" keepAlive="1" name="Consulta - Log_salas (8)" description="Conexão com a consulta 'Log_salas (8)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (8)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (8)]"/>
   </connection>
-  <connection id="15" keepAlive="1" name="Consulta - Log_salas (9)" description="Conexão com a consulta 'Log_salas (9)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="15" xr16:uid="{00000000-0015-0000-FFFF-FFFF0E000000}" keepAlive="1" name="Consulta - Log_salas (9)" description="Conexão com a consulta 'Log_salas (9)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas (9)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas (9)]"/>
   </connection>
-  <connection id="16" keepAlive="1" name="Consulta - Log_salas 0822-23" description="Conexão com a consulta 'Log_salas 0822-23' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="16" xr16:uid="{00000000-0015-0000-FFFF-FFFF0F000000}" keepAlive="1" name="Consulta - Log_salas 0822-23" description="Conexão com a consulta 'Log_salas 0822-23' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas 0822-23&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas 0822-23]"/>
   </connection>
-  <connection id="17" keepAlive="1" name="Consulta - Log_salas 0986-22" description="Conexão com a consulta 'Log_salas 0986-22' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="17" xr16:uid="{00000000-0015-0000-FFFF-FFFF10000000}" keepAlive="1" name="Consulta - Log_salas 0986-22" description="Conexão com a consulta 'Log_salas 0986-22' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_salas 0986-22&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_salas 0986-22]"/>
   </connection>
-  <connection id="18" keepAlive="1" name="Consulta - Log_sensores (1)" description="Conexão com a consulta 'Log_sensores (1)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="18" xr16:uid="{00000000-0015-0000-FFFF-FFFF11000000}" keepAlive="1" name="Consulta - Log_sensores (1)" description="Conexão com a consulta 'Log_sensores (1)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_sensores (1)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_sensores (1)]"/>
   </connection>
-  <connection id="19" keepAlive="1" name="Consulta - Log_sensores (3)" description="Conexão com a consulta 'Log_sensores (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="19" xr16:uid="{00000000-0015-0000-FFFF-FFFF12000000}" keepAlive="1" name="Consulta - Log_sensores (3)" description="Conexão com a consulta 'Log_sensores (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_sensores (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_sensores (3)]"/>
   </connection>
-  <connection id="20" keepAlive="1" name="Consulta - Log_tubo" description="Conexão com a consulta 'Log_tubo' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="20" xr16:uid="{00000000-0015-0000-FFFF-FFFF13000000}" keepAlive="1" name="Consulta - Log_tubo" description="Conexão com a consulta 'Log_tubo' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Log_tubo;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo]"/>
   </connection>
-  <connection id="21" keepAlive="1" name="Consulta - Log_tubo - 0986-22" description="Conexão com a consulta 'Log_tubo - 0986-22' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="21" xr16:uid="{00000000-0015-0000-FFFF-FFFF14000000}" keepAlive="1" name="Consulta - Log_tubo - 0986-22" description="Conexão com a consulta 'Log_tubo - 0986-22' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo - 0986-22&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo - 0986-22]"/>
   </connection>
-  <connection id="22" keepAlive="1" name="Consulta - Log_tubo (1)" description="Conexão com a consulta 'Log_tubo (1)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="22" xr16:uid="{00000000-0015-0000-FFFF-FFFF15000000}" keepAlive="1" name="Consulta - Log_tubo (1)" description="Conexão com a consulta 'Log_tubo (1)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo (1)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo (1)]"/>
   </connection>
-  <connection id="23" keepAlive="1" name="Consulta - Log_tubo (2)" description="Conexão com a consulta 'Log_tubo (2)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="23" xr16:uid="{00000000-0015-0000-FFFF-FFFF16000000}" keepAlive="1" name="Consulta - Log_tubo (2)" description="Conexão com a consulta 'Log_tubo (2)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo (2)]"/>
   </connection>
-  <connection id="24" keepAlive="1" name="Consulta - Log_tubo (3)" description="Conexão com a consulta 'Log_tubo (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="24" xr16:uid="{00000000-0015-0000-FFFF-FFFF17000000}" keepAlive="1" name="Consulta - Log_tubo (3)" description="Conexão com a consulta 'Log_tubo (3)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo (3)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo (3)]"/>
   </connection>
-  <connection id="25" keepAlive="1" name="Consulta - Log_tubo (4)" description="Conexão com a consulta 'Log_tubo (4)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="25" xr16:uid="{00000000-0015-0000-FFFF-FFFF18000000}" keepAlive="1" name="Consulta - Log_tubo (4)" description="Conexão com a consulta 'Log_tubo (4)' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo (4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo (4)]"/>
   </connection>
-  <connection id="26" keepAlive="1" name="Consulta - Log_tubo (5)" description="Ligação à consulta 'Log_tubo (5)' no livro." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="26" xr16:uid="{00000000-0015-0000-FFFF-FFFF19000000}" keepAlive="1" name="Consulta - Log_tubo (5)" description="Ligação à consulta 'Log_tubo (5)' no livro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo (5)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo (5)]"/>
   </connection>
-  <connection id="27" keepAlive="1" name="Consulta - Log_tubo 0822 - 23" description="Conexão com a consulta 'Log_tubo 0822 - 23' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="27" xr16:uid="{00000000-0015-0000-FFFF-FFFF1A000000}" keepAlive="1" name="Consulta - Log_tubo 0822 - 23" description="Conexão com a consulta 'Log_tubo 0822 - 23' na pasta de trabalho." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Log_tubo 0822 - 23&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Log_tubo 0822 - 23]"/>
   </connection>
 </connections>
@@ -253,7 +254,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -883,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -926,9 +927,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -959,64 +958,148 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1061,6 +1144,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1073,139 +1159,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1245,7 +1238,7 @@
         <xdr:cNvPr id="6" name="Imagem 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022A7451-D9D1-4862-B24F-133568D76677}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022A7451-D9D1-4862-B24F-133568D76677}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1283,7 @@
         <xdr:cNvPr id="7" name="CaixaDeTexto 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38956A7C-ABFA-46DF-B5FF-C318769B3683}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38956A7C-ABFA-46DF-B5FF-C318769B3683}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1382,7 +1375,7 @@
         <xdr:cNvPr id="8" name="Imagem 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{146B9758-A851-4C10-ABA8-1092CDD61F29}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{146B9758-A851-4C10-ABA8-1092CDD61F29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1432,7 +1425,7 @@
         <xdr:cNvPr id="11" name="Imagem 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68C2820B-EAC3-4928-B59E-5DAE5B48B1F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68C2820B-EAC3-4928-B59E-5DAE5B48B1F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1477,7 +1470,7 @@
         <xdr:cNvPr id="13" name="CaixaDeTexto 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE23EA4-A279-403F-A852-1A021C18C9E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FE23EA4-A279-403F-A852-1A021C18C9E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1569,7 +1562,7 @@
         <xdr:cNvPr id="14" name="Imagem 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C342430B-A2F5-4477-BD72-82FA412F8CE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C342430B-A2F5-4477-BD72-82FA412F8CE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1612,7 @@
         <xdr:cNvPr id="15" name="Imagem 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{863B3085-0C32-4D87-AE81-5B280F9CD850}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{863B3085-0C32-4D87-AE81-5B280F9CD850}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1664,7 +1657,7 @@
         <xdr:cNvPr id="16" name="CaixaDeTexto 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DA5A63A-B5DD-4EE1-A545-CE54D7151F1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DA5A63A-B5DD-4EE1-A545-CE54D7151F1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1756,7 +1749,7 @@
         <xdr:cNvPr id="17" name="Imagem 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E831530-6F05-4756-86F6-1625FD8B02C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E831530-6F05-4756-86F6-1625FD8B02C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,14 +2080,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1621"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -52352,375 +52345,375 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:J1621"/>
+  <autoFilter ref="B1:J1621" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A76" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="F93" sqref="F93"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A72" zoomScale="70" zoomScaleNormal="55" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" customWidth="1"/>
-    <col min="10" max="10" width="60.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="4.88671875" customWidth="1"/>
+    <col min="10" max="10" width="60.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A1" s="112"/>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="114"/>
-    </row>
-    <row r="2" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A2" s="86" t="s">
+    <row r="1" spans="1:10" ht="99.9" customHeight="1">
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="32" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="31" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="118"/>
-    </row>
-    <row r="3" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A3" s="115" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+    </row>
+    <row r="3" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A3" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="111"/>
-    </row>
-    <row r="4" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A4" s="86" t="s">
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="45"/>
+    </row>
+    <row r="4" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="110" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="111"/>
-    </row>
-    <row r="5" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A5" s="94" t="s">
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45"/>
+    </row>
+    <row r="5" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A5" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="96"/>
-    </row>
-    <row r="6" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A6" s="86" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+    </row>
+    <row r="6" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="30" t="s">
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="76"/>
-    </row>
-    <row r="7" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A7" s="103" t="s">
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="52"/>
+    </row>
+    <row r="7" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A7" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="104"/>
-      <c r="I7" s="104"/>
-      <c r="J7" s="105"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="8" spans="1:10" ht="33" customHeight="1">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="57"/>
+      <c r="C8" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="31" t="s">
+      <c r="D8" s="32"/>
+      <c r="E8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="31" t="s">
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A9" s="37"/>
-      <c r="B9" s="106"/>
-      <c r="C9" s="33" t="s">
+      <c r="I8" s="46"/>
+      <c r="J8" s="60"/>
+    </row>
+    <row r="9" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A9" s="56"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
-      <c r="H9" s="36" t="s">
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="108"/>
-      <c r="J9" s="109"/>
-    </row>
-    <row r="10" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A10" s="97" t="s">
+      <c r="I9" s="62"/>
+      <c r="J9" s="63"/>
+    </row>
+    <row r="10" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A10" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A11" s="97"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="90"/>
-    </row>
-    <row r="12" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A12" s="97"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="90"/>
-    </row>
-    <row r="13" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A13" s="97"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="90"/>
-    </row>
-    <row r="14" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A14" s="97"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="90"/>
-    </row>
-    <row r="15" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A15" s="97"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="90"/>
-    </row>
-    <row r="16" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A16" s="97"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="89"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="89"/>
-      <c r="J16" s="90"/>
-    </row>
-    <row r="17" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A17" s="97"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="89"/>
-      <c r="J17" s="90"/>
-    </row>
-    <row r="18" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A18" s="97"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="89"/>
-      <c r="J18" s="90"/>
-    </row>
-    <row r="19" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A19" s="97"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
-      <c r="J19" s="90"/>
-    </row>
-    <row r="20" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A20" s="97"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="90"/>
-    </row>
-    <row r="21" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A21" s="97"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
-      <c r="J21" s="90"/>
-    </row>
-    <row r="22" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A22" s="97"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="89"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="90"/>
-    </row>
-    <row r="23" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A23" s="97"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="90"/>
-    </row>
-    <row r="24" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A24" s="97"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="89"/>
-      <c r="G24" s="89"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="89"/>
-      <c r="J24" s="90"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A11" s="64"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="70"/>
+    </row>
+    <row r="12" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A12" s="64"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="70"/>
+    </row>
+    <row r="13" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A13" s="64"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
+    </row>
+    <row r="14" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A14" s="64"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="70"/>
+    </row>
+    <row r="15" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A15" s="64"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
+    </row>
+    <row r="16" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A16" s="64"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="70"/>
+    </row>
+    <row r="17" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A17" s="64"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A18" s="64"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="19" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A19" s="64"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="70"/>
+    </row>
+    <row r="20" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A20" s="64"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="70"/>
+    </row>
+    <row r="21" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A21" s="64"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+    </row>
+    <row r="22" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A22" s="64"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="70"/>
+    </row>
+    <row r="23" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A23" s="64"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="70"/>
+    </row>
+    <row r="24" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A24" s="64"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="70"/>
     </row>
     <row r="25" spans="1:10" ht="217.5" customHeight="1">
-      <c r="A25" s="97"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="93"/>
-    </row>
-    <row r="26" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A26" s="97"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="73"/>
+    </row>
+    <row r="26" spans="1:10" ht="21.9" customHeight="1">
+      <c r="A26" s="64"/>
       <c r="B26" s="19" t="s">
         <v>28</v>
       </c>
@@ -52733,8 +52726,8 @@
       <c r="I26" s="14"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A27" s="97"/>
+    <row r="27" spans="1:10" ht="21.9" customHeight="1">
+      <c r="A27" s="64"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -52745,8 +52738,8 @@
       <c r="I27" s="14"/>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A28" s="97"/>
+    <row r="28" spans="1:10" ht="21.9" customHeight="1">
+      <c r="A28" s="64"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
@@ -52769,296 +52762,296 @@
       <c r="I29" s="17"/>
       <c r="J29" s="18"/>
     </row>
-    <row r="30" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A30" s="83"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="85"/>
+    <row r="30" spans="1:10" ht="99.9" customHeight="1">
+      <c r="A30" s="80"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="82"/>
     </row>
     <row r="31" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="99"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="100"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="67"/>
     </row>
     <row r="32" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="87"/>
-      <c r="C32" s="30" t="s">
+      <c r="B32" s="40"/>
+      <c r="C32" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="30" t="s">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="76"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="52"/>
     </row>
     <row r="33" spans="1:10" ht="36" customHeight="1">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="31" t="s">
+      <c r="B33" s="57"/>
+      <c r="C33" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="31" t="s">
+      <c r="D33" s="32"/>
+      <c r="E33" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="31" t="s">
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="60"/>
     </row>
     <row r="34" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="32" t="s">
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="31" t="s">
+      <c r="D34" s="32"/>
+      <c r="E34" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="31" t="s">
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I34" s="101"/>
-      <c r="J34" s="102"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="60"/>
     </row>
     <row r="35" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="26"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A36" s="58"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="90"/>
+      <c r="A36" s="84"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="70"/>
     </row>
     <row r="37" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A37" s="58"/>
-      <c r="B37" s="88"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="89"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="89"/>
-      <c r="J37" s="90"/>
+      <c r="A37" s="84"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="70"/>
     </row>
     <row r="38" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A38" s="58"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="90"/>
+      <c r="A38" s="84"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="70"/>
     </row>
     <row r="39" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A39" s="58"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="90"/>
+      <c r="A39" s="84"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="69"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="70"/>
     </row>
     <row r="40" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A40" s="58"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="89"/>
-      <c r="D40" s="89"/>
-      <c r="E40" s="89"/>
-      <c r="F40" s="89"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="89"/>
-      <c r="I40" s="89"/>
-      <c r="J40" s="90"/>
+      <c r="A40" s="84"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="70"/>
     </row>
     <row r="41" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A41" s="58"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="89"/>
-      <c r="D41" s="89"/>
-      <c r="E41" s="89"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="89"/>
-      <c r="I41" s="89"/>
-      <c r="J41" s="90"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="69"/>
+      <c r="J41" s="70"/>
     </row>
     <row r="42" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A42" s="58"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="89"/>
-      <c r="J42" s="90"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="70"/>
     </row>
     <row r="43" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A43" s="58"/>
-      <c r="B43" s="88"/>
-      <c r="C43" s="89"/>
-      <c r="D43" s="89"/>
-      <c r="E43" s="89"/>
-      <c r="F43" s="89"/>
-      <c r="G43" s="89"/>
-      <c r="H43" s="89"/>
-      <c r="I43" s="89"/>
-      <c r="J43" s="90"/>
+      <c r="A43" s="84"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="70"/>
     </row>
     <row r="44" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A44" s="58"/>
-      <c r="B44" s="88"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="90"/>
+      <c r="A44" s="84"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="70"/>
     </row>
     <row r="45" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A45" s="58"/>
-      <c r="B45" s="88"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="90"/>
+      <c r="A45" s="84"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="70"/>
     </row>
     <row r="46" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A46" s="58"/>
-      <c r="B46" s="88"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="89"/>
-      <c r="J46" s="90"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="70"/>
     </row>
     <row r="47" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A47" s="58"/>
-      <c r="B47" s="88"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="89"/>
-      <c r="G47" s="89"/>
-      <c r="H47" s="89"/>
-      <c r="I47" s="89"/>
-      <c r="J47" s="90"/>
+      <c r="A47" s="84"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="70"/>
     </row>
     <row r="48" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A48" s="58"/>
-      <c r="B48" s="88"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="89"/>
-      <c r="J48" s="90"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="68"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="70"/>
     </row>
     <row r="49" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A49" s="58"/>
-      <c r="B49" s="88"/>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="90"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="70"/>
     </row>
     <row r="50" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A50" s="58"/>
-      <c r="B50" s="88"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="89"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="89"/>
-      <c r="J50" s="90"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="68"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="70"/>
     </row>
     <row r="51" spans="1:10" ht="168.75" customHeight="1">
-      <c r="A51" s="58"/>
-      <c r="B51" s="91"/>
-      <c r="C51" s="92"/>
-      <c r="D51" s="92"/>
-      <c r="E51" s="92"/>
-      <c r="F51" s="92"/>
-      <c r="G51" s="92"/>
-      <c r="H51" s="92"/>
-      <c r="I51" s="92"/>
-      <c r="J51" s="93"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="71"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="73"/>
     </row>
     <row r="52" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A52" s="58"/>
+      <c r="A52" s="84"/>
       <c r="B52" s="23" t="s">
         <v>28</v>
       </c>
@@ -53072,7 +53065,7 @@
       <c r="J52" s="10"/>
     </row>
     <row r="53" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A53" s="58"/>
+      <c r="A53" s="84"/>
       <c r="B53" s="7"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -53084,7 +53077,7 @@
       <c r="J53" s="10"/>
     </row>
     <row r="54" spans="1:10" ht="26.1" customHeight="1">
-      <c r="A54" s="59"/>
+      <c r="A54" s="85"/>
       <c r="B54" s="11"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -53095,344 +53088,344 @@
       <c r="I54" s="21"/>
       <c r="J54" s="22"/>
     </row>
-    <row r="55" spans="1:10" ht="24.95" customHeight="1" thickBot="1">
-      <c r="A55" s="77"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="79"/>
-    </row>
-    <row r="56" spans="1:10" ht="99.95" customHeight="1">
-      <c r="A56" s="80"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="81"/>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="81"/>
-      <c r="G56" s="81"/>
-      <c r="H56" s="81"/>
-      <c r="I56" s="81"/>
-      <c r="J56" s="82"/>
-    </row>
-    <row r="57" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A57" s="94" t="s">
+    <row r="55" spans="1:10" ht="24.9" customHeight="1" thickBot="1">
+      <c r="A55" s="74"/>
+      <c r="B55" s="75"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="76"/>
+    </row>
+    <row r="56" spans="1:10" ht="99.9" customHeight="1">
+      <c r="A56" s="77"/>
+      <c r="B56" s="78"/>
+      <c r="C56" s="78"/>
+      <c r="D56" s="78"/>
+      <c r="E56" s="78"/>
+      <c r="F56" s="78"/>
+      <c r="G56" s="78"/>
+      <c r="H56" s="78"/>
+      <c r="I56" s="78"/>
+      <c r="J56" s="79"/>
+    </row>
+    <row r="57" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A57" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="95"/>
-      <c r="C57" s="95"/>
-      <c r="D57" s="95"/>
-      <c r="E57" s="95"/>
-      <c r="F57" s="95"/>
-      <c r="G57" s="95"/>
-      <c r="H57" s="95"/>
-      <c r="I57" s="95"/>
-      <c r="J57" s="96"/>
-    </row>
-    <row r="58" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A58" s="86" t="s">
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="51"/>
+    </row>
+    <row r="58" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A58" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="87"/>
-      <c r="C58" s="30" t="s">
+      <c r="B58" s="40"/>
+      <c r="C58" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="30" t="s">
+      <c r="D58" s="43"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="76"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="52"/>
     </row>
     <row r="59" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="31" t="s">
+      <c r="B59" s="57"/>
+      <c r="C59" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="34"/>
-      <c r="E59" s="31" t="s">
+      <c r="D59" s="32"/>
+      <c r="E59" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="31" t="s">
+      <c r="F59" s="59"/>
+      <c r="G59" s="59"/>
+      <c r="H59" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I59" s="40"/>
-      <c r="J59" s="41"/>
-    </row>
-    <row r="60" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A60" s="37"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="32" t="s">
+      <c r="I59" s="114"/>
+      <c r="J59" s="115"/>
+    </row>
+    <row r="60" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A60" s="56"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="34"/>
-      <c r="E60" s="31" t="s">
+      <c r="D60" s="32"/>
+      <c r="E60" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="31" t="s">
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I60" s="42"/>
-      <c r="J60" s="43"/>
-    </row>
-    <row r="61" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A61" s="57" t="s">
+      <c r="I60" s="46"/>
+      <c r="J60" s="60"/>
+    </row>
+    <row r="61" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A61" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
-      <c r="I61" s="28"/>
-      <c r="J61" s="29"/>
-    </row>
-    <row r="62" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A62" s="58"/>
-      <c r="B62" s="44"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="45"/>
-      <c r="I62" s="45"/>
-      <c r="J62" s="46"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="27"/>
+    </row>
+    <row r="62" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A62" s="84"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="103"/>
+      <c r="D62" s="103"/>
+      <c r="E62" s="103"/>
+      <c r="F62" s="103"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="103"/>
+      <c r="I62" s="103"/>
+      <c r="J62" s="104"/>
     </row>
     <row r="63" spans="1:10" ht="24" customHeight="1">
-      <c r="A63" s="58"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="46"/>
-    </row>
-    <row r="64" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A64" s="58"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="45"/>
-      <c r="H64" s="45"/>
-      <c r="I64" s="45"/>
-      <c r="J64" s="46"/>
-    </row>
-    <row r="65" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A65" s="58"/>
-      <c r="B65" s="44"/>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
-      <c r="F65" s="45"/>
-      <c r="G65" s="45"/>
-      <c r="H65" s="45"/>
-      <c r="I65" s="45"/>
-      <c r="J65" s="46"/>
+      <c r="A63" s="84"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="103"/>
+      <c r="E63" s="103"/>
+      <c r="F63" s="103"/>
+      <c r="G63" s="103"/>
+      <c r="H63" s="103"/>
+      <c r="I63" s="103"/>
+      <c r="J63" s="104"/>
+    </row>
+    <row r="64" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A64" s="84"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
+      <c r="E64" s="103"/>
+      <c r="F64" s="103"/>
+      <c r="G64" s="103"/>
+      <c r="H64" s="103"/>
+      <c r="I64" s="103"/>
+      <c r="J64" s="104"/>
+    </row>
+    <row r="65" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A65" s="84"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="103"/>
+      <c r="D65" s="103"/>
+      <c r="E65" s="103"/>
+      <c r="F65" s="103"/>
+      <c r="G65" s="103"/>
+      <c r="H65" s="103"/>
+      <c r="I65" s="103"/>
+      <c r="J65" s="104"/>
     </row>
     <row r="66" spans="1:10" ht="24" customHeight="1">
-      <c r="A66" s="58"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="45"/>
-      <c r="J66" s="46"/>
-    </row>
-    <row r="67" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A67" s="58"/>
-      <c r="B67" s="44"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="45"/>
-      <c r="J67" s="46"/>
-    </row>
-    <row r="68" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A68" s="58"/>
-      <c r="B68" s="44"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="45"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="45"/>
-      <c r="J68" s="46"/>
-    </row>
-    <row r="69" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A69" s="58"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="45"/>
-      <c r="J69" s="46"/>
+      <c r="A66" s="84"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="103"/>
+      <c r="D66" s="103"/>
+      <c r="E66" s="103"/>
+      <c r="F66" s="103"/>
+      <c r="G66" s="103"/>
+      <c r="H66" s="103"/>
+      <c r="I66" s="103"/>
+      <c r="J66" s="104"/>
+    </row>
+    <row r="67" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A67" s="84"/>
+      <c r="B67" s="102"/>
+      <c r="C67" s="103"/>
+      <c r="D67" s="103"/>
+      <c r="E67" s="103"/>
+      <c r="F67" s="103"/>
+      <c r="G67" s="103"/>
+      <c r="H67" s="103"/>
+      <c r="I67" s="103"/>
+      <c r="J67" s="104"/>
+    </row>
+    <row r="68" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A68" s="84"/>
+      <c r="B68" s="102"/>
+      <c r="C68" s="103"/>
+      <c r="D68" s="103"/>
+      <c r="E68" s="103"/>
+      <c r="F68" s="103"/>
+      <c r="G68" s="103"/>
+      <c r="H68" s="103"/>
+      <c r="I68" s="103"/>
+      <c r="J68" s="104"/>
+    </row>
+    <row r="69" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A69" s="84"/>
+      <c r="B69" s="102"/>
+      <c r="C69" s="103"/>
+      <c r="D69" s="103"/>
+      <c r="E69" s="103"/>
+      <c r="F69" s="103"/>
+      <c r="G69" s="103"/>
+      <c r="H69" s="103"/>
+      <c r="I69" s="103"/>
+      <c r="J69" s="104"/>
     </row>
     <row r="70" spans="1:10" ht="24" customHeight="1">
-      <c r="A70" s="58"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="45"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
-      <c r="F70" s="45"/>
-      <c r="G70" s="45"/>
-      <c r="H70" s="45"/>
-      <c r="I70" s="45"/>
-      <c r="J70" s="46"/>
-    </row>
-    <row r="71" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A71" s="58"/>
-      <c r="B71" s="44"/>
-      <c r="C71" s="45"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="45"/>
-      <c r="H71" s="45"/>
-      <c r="I71" s="45"/>
-      <c r="J71" s="46"/>
-    </row>
-    <row r="72" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A72" s="58"/>
-      <c r="B72" s="44"/>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="45"/>
-      <c r="J72" s="46"/>
-    </row>
-    <row r="73" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A73" s="58"/>
-      <c r="B73" s="44"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="45"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="45"/>
-      <c r="J73" s="46"/>
-    </row>
-    <row r="74" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A74" s="58"/>
-      <c r="B74" s="44"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="45"/>
-      <c r="J74" s="46"/>
-    </row>
-    <row r="75" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A75" s="58"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="45"/>
-      <c r="H75" s="45"/>
-      <c r="I75" s="45"/>
-      <c r="J75" s="46"/>
-    </row>
-    <row r="76" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A76" s="58"/>
-      <c r="B76" s="44"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="J76" s="46"/>
-    </row>
-    <row r="77" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A77" s="58"/>
-      <c r="B77" s="44"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="45"/>
-      <c r="J77" s="46"/>
-    </row>
-    <row r="78" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A78" s="58"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-      <c r="J78" s="46"/>
-    </row>
-    <row r="79" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A79" s="58"/>
-      <c r="B79" s="44"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="45"/>
-      <c r="I79" s="45"/>
-      <c r="J79" s="46"/>
+      <c r="A70" s="84"/>
+      <c r="B70" s="102"/>
+      <c r="C70" s="103"/>
+      <c r="D70" s="103"/>
+      <c r="E70" s="103"/>
+      <c r="F70" s="103"/>
+      <c r="G70" s="103"/>
+      <c r="H70" s="103"/>
+      <c r="I70" s="103"/>
+      <c r="J70" s="104"/>
+    </row>
+    <row r="71" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A71" s="84"/>
+      <c r="B71" s="102"/>
+      <c r="C71" s="103"/>
+      <c r="D71" s="103"/>
+      <c r="E71" s="103"/>
+      <c r="F71" s="103"/>
+      <c r="G71" s="103"/>
+      <c r="H71" s="103"/>
+      <c r="I71" s="103"/>
+      <c r="J71" s="104"/>
+    </row>
+    <row r="72" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A72" s="84"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="103"/>
+      <c r="D72" s="103"/>
+      <c r="E72" s="103"/>
+      <c r="F72" s="103"/>
+      <c r="G72" s="103"/>
+      <c r="H72" s="103"/>
+      <c r="I72" s="103"/>
+      <c r="J72" s="104"/>
+    </row>
+    <row r="73" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A73" s="84"/>
+      <c r="B73" s="102"/>
+      <c r="C73" s="103"/>
+      <c r="D73" s="103"/>
+      <c r="E73" s="103"/>
+      <c r="F73" s="103"/>
+      <c r="G73" s="103"/>
+      <c r="H73" s="103"/>
+      <c r="I73" s="103"/>
+      <c r="J73" s="104"/>
+    </row>
+    <row r="74" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A74" s="84"/>
+      <c r="B74" s="102"/>
+      <c r="C74" s="103"/>
+      <c r="D74" s="103"/>
+      <c r="E74" s="103"/>
+      <c r="F74" s="103"/>
+      <c r="G74" s="103"/>
+      <c r="H74" s="103"/>
+      <c r="I74" s="103"/>
+      <c r="J74" s="104"/>
+    </row>
+    <row r="75" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A75" s="84"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="103"/>
+      <c r="D75" s="103"/>
+      <c r="E75" s="103"/>
+      <c r="F75" s="103"/>
+      <c r="G75" s="103"/>
+      <c r="H75" s="103"/>
+      <c r="I75" s="103"/>
+      <c r="J75" s="104"/>
+    </row>
+    <row r="76" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A76" s="84"/>
+      <c r="B76" s="102"/>
+      <c r="C76" s="103"/>
+      <c r="D76" s="103"/>
+      <c r="E76" s="103"/>
+      <c r="F76" s="103"/>
+      <c r="G76" s="103"/>
+      <c r="H76" s="103"/>
+      <c r="I76" s="103"/>
+      <c r="J76" s="104"/>
+    </row>
+    <row r="77" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A77" s="84"/>
+      <c r="B77" s="102"/>
+      <c r="C77" s="103"/>
+      <c r="D77" s="103"/>
+      <c r="E77" s="103"/>
+      <c r="F77" s="103"/>
+      <c r="G77" s="103"/>
+      <c r="H77" s="103"/>
+      <c r="I77" s="103"/>
+      <c r="J77" s="104"/>
+    </row>
+    <row r="78" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A78" s="84"/>
+      <c r="B78" s="102"/>
+      <c r="C78" s="103"/>
+      <c r="D78" s="103"/>
+      <c r="E78" s="103"/>
+      <c r="F78" s="103"/>
+      <c r="G78" s="103"/>
+      <c r="H78" s="103"/>
+      <c r="I78" s="103"/>
+      <c r="J78" s="104"/>
+    </row>
+    <row r="79" spans="1:10" ht="24.9" customHeight="1">
+      <c r="A79" s="84"/>
+      <c r="B79" s="102"/>
+      <c r="C79" s="103"/>
+      <c r="D79" s="103"/>
+      <c r="E79" s="103"/>
+      <c r="F79" s="103"/>
+      <c r="G79" s="103"/>
+      <c r="H79" s="103"/>
+      <c r="I79" s="103"/>
+      <c r="J79" s="104"/>
     </row>
     <row r="80" spans="1:10" ht="123.75" customHeight="1">
-      <c r="A80" s="58"/>
-      <c r="B80" s="47"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
-      <c r="F80" s="48"/>
-      <c r="G80" s="48"/>
-      <c r="H80" s="48"/>
-      <c r="I80" s="48"/>
-      <c r="J80" s="49"/>
+      <c r="A80" s="84"/>
+      <c r="B80" s="105"/>
+      <c r="C80" s="106"/>
+      <c r="D80" s="106"/>
+      <c r="E80" s="106"/>
+      <c r="F80" s="106"/>
+      <c r="G80" s="106"/>
+      <c r="H80" s="106"/>
+      <c r="I80" s="106"/>
+      <c r="J80" s="107"/>
     </row>
     <row r="81" spans="1:10" ht="24" customHeight="1">
-      <c r="A81" s="58"/>
+      <c r="A81" s="84"/>
       <c r="B81" s="19" t="s">
         <v>28</v>
       </c>
@@ -53446,7 +53439,7 @@
       <c r="J81" s="2"/>
     </row>
     <row r="82" spans="1:10" ht="24" customHeight="1">
-      <c r="A82" s="58"/>
+      <c r="A82" s="84"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -53458,7 +53451,7 @@
       <c r="J82" s="2"/>
     </row>
     <row r="83" spans="1:10" ht="24" customHeight="1">
-      <c r="A83" s="59"/>
+      <c r="A83" s="85"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -53469,111 +53462,118 @@
       <c r="I83" s="1"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A84" s="54"/>
-      <c r="B84" s="55"/>
-      <c r="C84" s="55"/>
-      <c r="D84" s="55"/>
-      <c r="E84" s="55"/>
-      <c r="F84" s="55"/>
-      <c r="G84" s="55"/>
-      <c r="H84" s="55"/>
-      <c r="I84" s="55"/>
-      <c r="J84" s="56"/>
+    <row r="84" spans="1:10" ht="21.9" customHeight="1">
+      <c r="A84" s="111"/>
+      <c r="B84" s="112"/>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
+      <c r="H84" s="112"/>
+      <c r="I84" s="112"/>
+      <c r="J84" s="113"/>
     </row>
     <row r="85" spans="1:10" hidden="1">
-      <c r="A85" s="50"/>
-      <c r="B85" s="51"/>
-      <c r="C85" s="51"/>
-      <c r="D85" s="51"/>
-      <c r="E85" s="51"/>
-      <c r="F85" s="51"/>
-      <c r="G85" s="51"/>
-      <c r="H85" s="51"/>
-      <c r="I85" s="51"/>
-      <c r="J85" s="52"/>
+      <c r="A85" s="108"/>
+      <c r="B85" s="109"/>
+      <c r="C85" s="109"/>
+      <c r="D85" s="109"/>
+      <c r="E85" s="109"/>
+      <c r="F85" s="109"/>
+      <c r="G85" s="109"/>
+      <c r="H85" s="109"/>
+      <c r="I85" s="109"/>
+      <c r="J85" s="110"/>
     </row>
     <row r="86" spans="1:10" hidden="1">
-      <c r="A86" s="50"/>
-      <c r="B86" s="51"/>
-      <c r="C86" s="51"/>
-      <c r="D86" s="51"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="51"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="51"/>
-      <c r="I86" s="51"/>
-      <c r="J86" s="52"/>
+      <c r="A86" s="108"/>
+      <c r="B86" s="109"/>
+      <c r="C86" s="109"/>
+      <c r="D86" s="109"/>
+      <c r="E86" s="109"/>
+      <c r="F86" s="109"/>
+      <c r="G86" s="109"/>
+      <c r="H86" s="109"/>
+      <c r="I86" s="109"/>
+      <c r="J86" s="110"/>
     </row>
     <row r="87" spans="1:10" hidden="1">
-      <c r="A87" s="50"/>
-      <c r="B87" s="51"/>
-      <c r="C87" s="51"/>
-      <c r="D87" s="51"/>
-      <c r="E87" s="51"/>
-      <c r="F87" s="51"/>
-      <c r="G87" s="51"/>
-      <c r="H87" s="51"/>
-      <c r="I87" s="53"/>
+      <c r="A87" s="108"/>
+      <c r="B87" s="109"/>
+      <c r="C87" s="109"/>
+      <c r="D87" s="109"/>
+      <c r="E87" s="109"/>
+      <c r="F87" s="109"/>
+      <c r="G87" s="109"/>
+      <c r="H87" s="109"/>
+      <c r="I87" s="97"/>
       <c r="J87" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="21.95" customHeight="1">
-      <c r="A88" s="60" t="s">
+    <row r="88" spans="1:10" ht="21.9" customHeight="1">
+      <c r="A88" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="B88" s="61"/>
-      <c r="C88" s="64"/>
-      <c r="D88" s="65"/>
-      <c r="E88" s="66"/>
-      <c r="F88" s="70" t="s">
+      <c r="B88" s="87"/>
+      <c r="C88" s="90"/>
+      <c r="D88" s="91"/>
+      <c r="E88" s="92"/>
+      <c r="F88" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="G88" s="53"/>
+      <c r="G88" s="97"/>
       <c r="H88" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I88" s="119"/>
-      <c r="J88" s="71"/>
-    </row>
-    <row r="89" spans="1:10" ht="21.95" customHeight="1" thickBot="1">
-      <c r="A89" s="62"/>
-      <c r="B89" s="63"/>
-      <c r="C89" s="67"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="73" t="s">
+      <c r="I88" s="35"/>
+      <c r="J88" s="98"/>
+    </row>
+    <row r="89" spans="1:10" ht="21.9" customHeight="1" thickBot="1">
+      <c r="A89" s="88"/>
+      <c r="B89" s="89"/>
+      <c r="C89" s="93"/>
+      <c r="D89" s="94"/>
+      <c r="E89" s="95"/>
+      <c r="F89" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="G89" s="74"/>
+      <c r="G89" s="101"/>
       <c r="H89" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I89" s="6"/>
-      <c r="J89" s="72"/>
+      <c r="J89" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A59:B60"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="B62:J80"/>
+    <mergeCell ref="A85:J85"/>
+    <mergeCell ref="A86:J86"/>
+    <mergeCell ref="A87:I87"/>
+    <mergeCell ref="A84:J84"/>
+    <mergeCell ref="A61:A83"/>
+    <mergeCell ref="A88:B89"/>
+    <mergeCell ref="C88:E89"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="J88:J89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="G58:J58"/>
+    <mergeCell ref="A55:J55"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="B36:J51"/>
+    <mergeCell ref="A35:A54"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D58:E58"/>
     <mergeCell ref="A10:A28"/>
     <mergeCell ref="A31:J31"/>
     <mergeCell ref="A33:B34"/>
@@ -53584,35 +53584,28 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="B11:J25"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="A55:J55"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="B36:J51"/>
-    <mergeCell ref="A35:A54"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="A88:B89"/>
-    <mergeCell ref="C88:E89"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="J88:J89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="B62:J80"/>
-    <mergeCell ref="A85:J85"/>
-    <mergeCell ref="A86:J86"/>
-    <mergeCell ref="A87:I87"/>
-    <mergeCell ref="A84:J84"/>
-    <mergeCell ref="A61:A83"/>
-    <mergeCell ref="A59:B60"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="29" max="16383" man="1"/>
     <brk id="55" max="16383" man="1"/>

</xml_diff>